<commit_message>
finished the ecoveg growth forms
</commit_message>
<xml_diff>
--- a/data/eco_veg_growth_forms.xlsx
+++ b/data/eco_veg_growth_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au763634_uni_au_dk/Documents/MappingPlants/01 Vegetation changes Kobbefjord/data/nmds_nero/nmds_nero/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1204941D-973C-0242-A4E9-D8F080CB1DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{1204941D-973C-0242-A4E9-D8F080CB1DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294DCED5-4BE1-7546-930E-7EB12AEEC37E}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="2000" windowWidth="27580" windowHeight="16940" activeTab="1" xr2:uid="{DAA8D5E6-146B-8A4E-9EEE-19939DB4FD57}"/>
+    <workbookView xWindow="3200" yWindow="2000" windowWidth="27580" windowHeight="16940" xr2:uid="{DAA8D5E6-146B-8A4E-9EEE-19939DB4FD57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="284">
   <si>
     <t>taxon_code</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>Liana - A woody, climbing plant that begins life as terrestrial seedlings but relies on external structural support for height growth during some part of its life (Gerwing 2004), typically exceeding 5 m in height or length at maturity. Non-woody climbers are treated as a type of "Herb."</t>
+  </si>
+  <si>
+    <t>gramnoid</t>
   </si>
 </sst>
 </file>
@@ -903,12 +906,42 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -923,9 +956,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1262,16 +1306,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1291,7 +1337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1302,13 +1348,13 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>283</v>
       </c>
       <c r="E2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1319,13 +1365,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1336,7 +1382,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E4" t="s">
         <v>218</v>
@@ -1352,8 +1398,11 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1370,7 +1419,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1379,6 +1428,9 @@
       </c>
       <c r="C7" t="s">
         <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1391,8 +1443,11 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1402,8 +1457,11 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1">
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1414,13 +1472,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1431,13 +1489,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E11" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1451,7 +1509,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1461,8 +1519,11 @@
       <c r="C13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" hidden="1">
+      <c r="D13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1537,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1490,7 +1551,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1504,7 +1565,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1528,8 +1589,11 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1543,7 +1607,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1557,7 +1621,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1571,7 +1635,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1581,8 +1645,11 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" hidden="1">
+      <c r="D22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1592,8 +1659,11 @@
       <c r="C23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1">
+      <c r="D23" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1607,7 +1677,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1631,8 +1701,11 @@
       <c r="C26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" hidden="1">
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1646,7 +1719,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1656,8 +1729,11 @@
       <c r="C28" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" hidden="1">
+      <c r="D28" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -1667,8 +1743,11 @@
       <c r="C29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" hidden="1">
+      <c r="D29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1692,8 +1771,11 @@
       <c r="C31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" hidden="1">
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1703,8 +1785,11 @@
       <c r="C32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" hidden="1">
+      <c r="D32" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1718,7 +1803,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1732,7 +1817,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1742,8 +1827,11 @@
       <c r="C35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" hidden="1">
+      <c r="D35" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -1757,7 +1845,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1781,8 +1869,11 @@
       <c r="C38" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1">
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -1796,12 +1887,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -1815,7 +1906,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1832,7 +1923,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -1842,8 +1933,11 @@
       <c r="C43" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1">
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -1853,8 +1947,11 @@
       <c r="C44" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1">
+      <c r="D44" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -1864,8 +1961,11 @@
       <c r="C45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" hidden="1">
+      <c r="D45" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -1875,8 +1975,11 @@
       <c r="C46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1">
+      <c r="D46" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -1890,7 +1993,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -1904,7 +2007,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>101</v>
       </c>
@@ -1914,8 +2017,11 @@
       <c r="C49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" hidden="1">
+      <c r="D49" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -1939,6 +2045,9 @@
       <c r="C51" t="s">
         <v>15</v>
       </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
@@ -1950,8 +2059,11 @@
       <c r="C52" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" hidden="1">
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1961,8 +2073,11 @@
       <c r="C53" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" hidden="1">
+      <c r="D53" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -1971,6 +2086,9 @@
       </c>
       <c r="C54" t="s">
         <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1983,8 +2101,11 @@
       <c r="C55" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" hidden="1">
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -2001,7 +2122,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2011,8 +2132,11 @@
       <c r="C57" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" hidden="1">
+      <c r="D57" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -2026,7 +2150,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -2036,8 +2160,11 @@
       <c r="C59" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" hidden="1">
+      <c r="D59" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -2051,7 +2178,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -2065,7 +2192,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>127</v>
       </c>
@@ -2079,7 +2206,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>129</v>
       </c>
@@ -2093,7 +2220,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -2107,7 +2234,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -2116,6 +2243,9 @@
       </c>
       <c r="C65" t="s">
         <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2128,8 +2258,11 @@
       <c r="C66" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1">
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>137</v>
       </c>
@@ -2146,7 +2279,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -2160,7 +2293,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -2174,7 +2307,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -2184,8 +2317,11 @@
       <c r="C70" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" hidden="1">
+      <c r="D70" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -2199,7 +2335,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -2209,8 +2345,11 @@
       <c r="C72" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" hidden="1">
+      <c r="D72" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -2224,7 +2363,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>151</v>
       </c>
@@ -2238,7 +2377,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -2252,7 +2391,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -2266,7 +2405,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -2280,7 +2419,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -2290,8 +2429,11 @@
       <c r="C78" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" hidden="1">
+      <c r="D78" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -2301,8 +2443,11 @@
       <c r="C79" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" hidden="1">
+      <c r="D79" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -2312,8 +2457,11 @@
       <c r="C80" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" hidden="1">
+      <c r="D80" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>165</v>
       </c>
@@ -2323,8 +2471,11 @@
       <c r="C81" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" hidden="1">
+      <c r="D81" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -2338,7 +2489,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>169</v>
       </c>
@@ -2348,8 +2499,11 @@
       <c r="C83" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" hidden="1">
+      <c r="D83" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>171</v>
       </c>
@@ -2359,8 +2513,11 @@
       <c r="C84" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" hidden="1">
+      <c r="D84" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -2370,8 +2527,11 @@
       <c r="C85" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" hidden="1">
+      <c r="D85" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -2381,8 +2541,11 @@
       <c r="C86" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" hidden="1">
+      <c r="D86" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -2392,8 +2555,11 @@
       <c r="C87" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" hidden="1">
+      <c r="D87" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>179</v>
       </c>
@@ -2407,7 +2573,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>181</v>
       </c>
@@ -2421,7 +2587,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>183</v>
       </c>
@@ -2431,8 +2597,11 @@
       <c r="C90" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" hidden="1">
+      <c r="D90" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>185</v>
       </c>
@@ -2449,7 +2618,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -2463,7 +2632,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>189</v>
       </c>
@@ -2477,7 +2646,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>191</v>
       </c>
@@ -2491,12 +2660,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>194</v>
       </c>
@@ -2506,8 +2675,11 @@
       <c r="C96" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" hidden="1">
+      <c r="D96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>196</v>
       </c>
@@ -2517,8 +2689,11 @@
       <c r="C97" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" hidden="1">
+      <c r="D97" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>198</v>
       </c>
@@ -2532,7 +2707,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>200</v>
       </c>
@@ -2542,8 +2717,11 @@
       <c r="C99" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" hidden="1">
+      <c r="D99" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>202</v>
       </c>
@@ -2557,7 +2735,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>204</v>
       </c>
@@ -2565,7 +2743,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>205</v>
       </c>
@@ -2575,8 +2753,11 @@
       <c r="C102" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" hidden="1">
+      <c r="D102" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>207</v>
       </c>
@@ -2590,7 +2771,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>209</v>
       </c>
@@ -2600,8 +2781,11 @@
       <c r="C104" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" hidden="1">
+      <c r="D104" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>211</v>
       </c>
@@ -2616,13 +2800,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E105" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="shrub"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E105" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2630,344 +2808,375 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C48A9B-7EAF-A64F-95F6-76A05247B70E}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="256" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="225.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.796875" customWidth="1"/>
+    <col min="4" max="4" width="256" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="225.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>221</v>
       </c>
       <c r="B1" t="s">
         <v>222</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
-      <c r="A19" t="s">
+    <row r="19" spans="1:4" ht="15">
+      <c r="A19" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" ht="15">
+      <c r="A29" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="A30" t="s">
+    <row r="30" spans="1:4" ht="15">
+      <c r="A30" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="7"/>
+      <c r="D30" s="8" t="s">
         <v>282</v>
       </c>
     </row>

</xml_diff>

<commit_message>
importing the functional types for analysis
</commit_message>
<xml_diff>
--- a/data/eco_veg_growth_forms.xlsx
+++ b/data/eco_veg_growth_forms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au763634_uni_au_dk/Documents/MappingPlants/01 Vegetation changes Kobbefjord/data/nmds_nero/nmds_nero/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibdj/Library/CloudStorage/OneDrive-Aarhusuniversitet/MappingPlants/01 Vegetation changes Kobbefjord/data/nmds_nero/nmds_nero/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{1204941D-973C-0242-A4E9-D8F080CB1DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294DCED5-4BE1-7546-930E-7EB12AEEC37E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1129EB1E-92E2-854F-9AEC-40876981C4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2000" windowWidth="27580" windowHeight="16940" xr2:uid="{DAA8D5E6-146B-8A4E-9EEE-19939DB4FD57}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="287">
   <si>
     <t>taxon_code</t>
   </si>
@@ -892,6 +892,15 @@
   </si>
   <si>
     <t>gramnoid</t>
+  </si>
+  <si>
+    <t>Bryophyte</t>
+  </si>
+  <si>
+    <t>Lichen</t>
+  </si>
+  <si>
+    <t>Rock</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1407,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>284</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1452,7 +1461,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>286</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -1483,7 +1492,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>285</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
refined functional types, the different levels
</commit_message>
<xml_diff>
--- a/data/eco_veg_growth_forms.xlsx
+++ b/data/eco_veg_growth_forms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au763634_uni_au_dk/Documents/MappingPlants/01 Vegetation changes Kobbefjord/data/nmds_nero/nmds_nero/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au763634_uni_au_dk/Documents/MappingPlants/01 Vegetation changes Kobbefjord/data/nero_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{1129EB1E-92E2-854F-9AEC-40876981C4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D3CB5E2-5D31-ED44-87FF-6794C7DD0628}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{84C7C7DF-45BF-5946-954F-E4B9701F5DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C24CEA8-2B3A-9B49-8CB9-1F1CF149CA67}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="2000" windowWidth="27580" windowHeight="16940" xr2:uid="{DAA8D5E6-146B-8A4E-9EEE-19939DB4FD57}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="286">
   <si>
     <t>taxon_code</t>
   </si>
@@ -111,9 +111,6 @@
     <t>rock</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>stereo</t>
   </si>
   <si>
@@ -684,15 +681,9 @@
     <t>herb</t>
   </si>
   <si>
-    <t>herb_forb_e</t>
-  </si>
-  <si>
     <t>herb_graminoid</t>
   </si>
   <si>
-    <t>non_vascular</t>
-  </si>
-  <si>
     <t>non_vascular_lichen</t>
   </si>
   <si>
@@ -904,6 +895,9 @@
   </si>
   <si>
     <t>shrub_decidous</t>
+  </si>
+  <si>
+    <t>non_vascular_bryo</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1351,16 +1345,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>280</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E2" t="s">
         <v>215</v>
@@ -1368,1487 +1362,1725 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>286</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>283</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E7" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>285</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>212</v>
+      </c>
+      <c r="E9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E12" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>282</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E15" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E16" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E17" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E18" t="s">
-        <v>286</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E19" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E20" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E21" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E22" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E23" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E24" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E25" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E26" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E27" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E28" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E29" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E30" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E31" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E32" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E33" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E34" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E35" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E36" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E37" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E38" t="s">
-        <v>286</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E39" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>155</v>
+      </c>
+      <c r="B40" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>212</v>
+      </c>
+      <c r="E40" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E41" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E43" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>183</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D44" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E44" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D45" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E45" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>187</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E46" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E47" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E48" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>282</v>
+        <v>212</v>
+      </c>
+      <c r="E49" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="E50" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>212</v>
       </c>
       <c r="E51" t="s">
-        <v>287</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>279</v>
       </c>
       <c r="E52" t="s">
-        <v>286</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E53" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E54" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>279</v>
       </c>
       <c r="E55" t="s">
-        <v>286</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
+        <v>279</v>
+      </c>
+      <c r="E56" t="s">
         <v>213</v>
-      </c>
-      <c r="E56" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E57" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
+        <v>279</v>
+      </c>
+      <c r="E58" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
         <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E59" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D60" t="s">
+        <v>279</v>
+      </c>
+      <c r="E60" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D61" t="s">
+        <v>279</v>
+      </c>
+      <c r="E61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D62" t="s">
+        <v>279</v>
+      </c>
+      <c r="E62" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
+        <v>279</v>
+      </c>
+      <c r="E63" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
+        <v>279</v>
+      </c>
+      <c r="E64" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E65" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>279</v>
       </c>
       <c r="E66" t="s">
-        <v>286</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E67" t="s">
         <v>213</v>
-      </c>
-      <c r="E67" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D68" t="s">
+        <v>279</v>
+      </c>
+      <c r="E68" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D69" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" t="s">
         <v>142</v>
-      </c>
-      <c r="B70" t="s">
-        <v>143</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E70" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D71" t="s">
+        <v>279</v>
+      </c>
+      <c r="E71" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C72" t="s">
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E72" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="C73" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D73" t="s">
+        <v>279</v>
+      </c>
+      <c r="E73" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D74" t="s">
+        <v>279</v>
+      </c>
+      <c r="E74" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C75" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D75" t="s">
+        <v>279</v>
+      </c>
+      <c r="E75" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="C76" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
+        <v>279</v>
+      </c>
+      <c r="E76" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
+        <v>279</v>
+      </c>
+      <c r="E77" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
       </c>
       <c r="D78" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E78" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
       </c>
       <c r="D79" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E79" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B80" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E80" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="C81" t="s">
         <v>7</v>
       </c>
       <c r="D81" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E81" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="B82" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D82" t="s">
+        <v>279</v>
+      </c>
+      <c r="E82" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E83" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="B84" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E84" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E85" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="C86" t="s">
         <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E86" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>176</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>177</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>282</v>
+        <v>214</v>
+      </c>
+      <c r="E87" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>178</v>
+        <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>179</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D88" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="E88" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>181</v>
+        <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="E89" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>182</v>
+        <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>183</v>
+        <v>281</v>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>282</v>
+        <v>214</v>
+      </c>
+      <c r="E90" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>184</v>
-      </c>
-      <c r="B91" t="s">
-        <v>185</v>
-      </c>
-      <c r="C91" t="s">
-        <v>28</v>
-      </c>
-      <c r="D91" t="s">
-        <v>213</v>
-      </c>
-      <c r="E91" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>186</v>
+        <v>22</v>
       </c>
       <c r="B92" t="s">
-        <v>187</v>
+        <v>282</v>
       </c>
       <c r="C92" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D92" t="s">
-        <v>213</v>
+        <v>22</v>
+      </c>
+      <c r="E92" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>188</v>
+        <v>13</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
+        <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D93" t="s">
-        <v>213</v>
+        <v>15</v>
+      </c>
+      <c r="E93" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>190</v>
+        <v>20</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D94" t="s">
-        <v>213</v>
+        <v>15</v>
+      </c>
+      <c r="E94" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>192</v>
+        <v>38</v>
+      </c>
+      <c r="B95" t="s">
+        <v>39</v>
+      </c>
+      <c r="C95" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>193</v>
+        <v>54</v>
       </c>
       <c r="B96" t="s">
-        <v>194</v>
+        <v>55</v>
       </c>
       <c r="C96" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D96" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E96" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>195</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>196</v>
+        <v>65</v>
       </c>
       <c r="C97" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D97" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E97" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>197</v>
+        <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
       <c r="C98" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D98" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E98" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>200</v>
+        <v>88</v>
       </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D99" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>201</v>
+        <v>103</v>
       </c>
       <c r="B100" t="s">
-        <v>202</v>
+        <v>104</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D100" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E100" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>203</v>
+        <v>105</v>
       </c>
       <c r="B101" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>106</v>
+      </c>
+      <c r="C101" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>111</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>112</v>
       </c>
       <c r="C102" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D102" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E102" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="B103" t="s">
-        <v>207</v>
+        <v>134</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D103" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+        <v>15</v>
+      </c>
+      <c r="E103" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>208</v>
-      </c>
-      <c r="B104" t="s">
-        <v>209</v>
-      </c>
-      <c r="C104" t="s">
-        <v>7</v>
-      </c>
-      <c r="D104" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>210</v>
-      </c>
-      <c r="B105" t="s">
-        <v>211</v>
-      </c>
-      <c r="C105" t="s">
-        <v>28</v>
-      </c>
-      <c r="D105" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E105" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}"/>
+  <autoFilter ref="A1:E105" xr:uid="{4EF2477A-3F92-C544-B07D-BB64AA107C04}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E105">
+      <sortCondition ref="C1:C105"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2873,359 +3105,359 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15">
       <c r="A19" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15">
       <c r="A29" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15">
       <c r="A30" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>